<commit_message>
trouble shooting data layers table
</commit_message>
<xml_diff>
--- a/region2017/reports/documents/LE/le_summary_tables.xlsx
+++ b/region2017/reports/documents/LE/le_summary_tables.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8360" yWindow="1260" windowWidth="25760" windowHeight="13740" tabRatio="500"/>
+    <workbookView xWindow="3040" yWindow="1260" windowWidth="25760" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="ECO" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="34">
   <si>
     <t>jobs_all</t>
   </si>
@@ -115,6 +116,21 @@
   </si>
   <si>
     <t>ocean jobs</t>
+  </si>
+  <si>
+    <t>rgn_id</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>total_revenue(adj with multipliers)</t>
+  </si>
+  <si>
+    <t>Hawaiʻi</t>
+  </si>
+  <si>
+    <t>Total Adjusted Revenue</t>
   </si>
 </sst>
 </file>
@@ -124,8 +140,8 @@
   <numFmts count="4">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -260,7 +276,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -275,14 +291,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
@@ -321,25 +337,39 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -629,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -713,7 +743,7 @@
         <v>9.5554300000000002E-3</v>
       </c>
       <c r="K2">
-        <f>E2/D2</f>
+        <f t="shared" ref="K2:K10" si="0">E2/D2</f>
         <v>1.4510081300813007E-3</v>
       </c>
       <c r="M2" s="7">
@@ -751,11 +781,11 @@
         <v>0.99044456999999997</v>
       </c>
       <c r="K3">
-        <f>E3/D3</f>
+        <f t="shared" si="0"/>
         <v>0.15622858536585366</v>
       </c>
       <c r="M3" s="7">
-        <f t="shared" ref="M3:M10" si="0">I3/D3</f>
+        <f t="shared" ref="M3:M10" si="1">I3/D3</f>
         <v>0.15767959349593497</v>
       </c>
     </row>
@@ -791,11 +821,11 @@
         <v>0.99127956100000003</v>
       </c>
       <c r="K4">
-        <f>E4/D4</f>
+        <f t="shared" si="0"/>
         <v>0.31838599373825921</v>
       </c>
       <c r="M4" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.31838599874765183</v>
       </c>
     </row>
@@ -831,11 +861,11 @@
         <v>1.2684389000000001E-2</v>
       </c>
       <c r="K5">
-        <f>E5/D5</f>
+        <f t="shared" si="0"/>
         <v>1.7114570637119112E-3</v>
       </c>
       <c r="M5" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.13111034238227148</v>
       </c>
     </row>
@@ -869,11 +899,11 @@
         <v>7.9493459999999995E-3</v>
       </c>
       <c r="K6">
-        <f>E6/D6</f>
+        <f t="shared" si="0"/>
         <v>1.0105529085872576E-3</v>
       </c>
       <c r="M6" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.13111034238227148</v>
       </c>
     </row>
@@ -907,11 +937,11 @@
         <v>5.4883280999999999E-2</v>
       </c>
       <c r="K7">
-        <f>E7/D7</f>
+        <f t="shared" si="0"/>
         <v>6.8957841551246539E-3</v>
       </c>
       <c r="M7" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.13111034238227148</v>
       </c>
     </row>
@@ -945,11 +975,11 @@
         <v>7.1853871999999999E-2</v>
       </c>
       <c r="K8">
-        <f>E8/D8</f>
+        <f t="shared" si="0"/>
         <v>9.1585329639889187E-3</v>
       </c>
       <c r="M8" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.13111034238227148</v>
       </c>
     </row>
@@ -983,11 +1013,11 @@
         <v>0.85262911299999999</v>
       </c>
       <c r="K9">
-        <f>E9/D9</f>
+        <f t="shared" si="0"/>
         <v>0.11233401462603879</v>
       </c>
       <c r="M9" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.13111034238227148</v>
       </c>
     </row>
@@ -1023,11 +1053,11 @@
         <v>1.0058294329999999</v>
       </c>
       <c r="K10">
-        <f>E10/D10</f>
+        <f t="shared" si="0"/>
         <v>0.15505985567010311</v>
       </c>
       <c r="M10" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.15505985272459499</v>
       </c>
     </row>
@@ -1077,6 +1107,10 @@
       <c r="F13" s="19">
         <v>38130</v>
       </c>
+      <c r="G13">
+        <f>D14/(SUM(D13:D14))</f>
+        <v>0.99079774308196256</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
@@ -1115,6 +1149,9 @@
       <c r="F15" s="19">
         <v>39042</v>
       </c>
+      <c r="G15">
+        <v>0.99</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
@@ -1207,6 +1244,10 @@
       <c r="F20" s="19">
         <v>45711</v>
       </c>
+      <c r="G20">
+        <f>D20/SUM(D16:D20)</f>
+        <v>0.85678988518025112</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
@@ -1226,6 +1267,9 @@
       </c>
       <c r="F21" s="22">
         <v>39059</v>
+      </c>
+      <c r="G21">
+        <v>0.99</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1236,13 +1280,13 @@
       <c r="B24" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="37" t="s">
+      <c r="D24" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="38" t="s">
+      <c r="E24" s="37" t="s">
         <v>26</v>
       </c>
       <c r="F24" s="8"/>
@@ -1266,11 +1310,11 @@
       <c r="D25" s="11">
         <v>0.15767959300000001</v>
       </c>
-      <c r="E25" s="35">
+      <c r="E25" s="34">
         <f>F25/1000000</f>
         <v>993.16020000000003</v>
       </c>
-      <c r="F25" s="33">
+      <c r="F25" s="32">
         <v>993160200</v>
       </c>
       <c r="H25" s="26" t="s">
@@ -1293,11 +1337,11 @@
       <c r="D26" s="11">
         <v>0.31838599899999998</v>
       </c>
-      <c r="E26" s="35">
-        <f t="shared" ref="E26:E28" si="1">F26/1000000</f>
+      <c r="E26" s="34">
+        <f t="shared" ref="E26:E28" si="2">F26/1000000</f>
         <v>2165.4666000000002</v>
       </c>
-      <c r="F26" s="33">
+      <c r="F26" s="32">
         <v>2165466600</v>
       </c>
       <c r="H26" s="26" t="s">
@@ -1320,11 +1364,11 @@
       <c r="D27" s="11">
         <v>0.13111034199999999</v>
       </c>
-      <c r="E27" s="35">
-        <f t="shared" si="1"/>
+      <c r="E27" s="34">
+        <f t="shared" si="2"/>
         <v>2700.0782399999998</v>
       </c>
-      <c r="F27" s="33">
+      <c r="F27" s="32">
         <v>2700078240</v>
       </c>
       <c r="H27" s="26" t="s">
@@ -1347,11 +1391,11 @@
       <c r="D28" s="14">
         <v>0.155059853</v>
       </c>
-      <c r="E28" s="36">
-        <f t="shared" si="1"/>
+      <c r="E28" s="35">
+        <f t="shared" si="2"/>
         <v>217.88976</v>
       </c>
-      <c r="F28" s="34">
+      <c r="F28" s="33">
         <v>217889760</v>
       </c>
       <c r="H28" s="28" t="s">
@@ -1362,10 +1406,10 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="40">
+      <c r="C29" s="39">
         <f>SUM(C25:C28)</f>
         <v>103427.15900000001</v>
       </c>
@@ -1373,13 +1417,13 @@
         <f>AVERAGE(D25:D28)</f>
         <v>0.19055894675000001</v>
       </c>
-      <c r="F29" s="39">
+      <c r="F29" s="38">
         <f>SUM(F25:F28)</f>
         <v>6076594800</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="40" t="s">
         <v>27</v>
       </c>
       <c r="C30">
@@ -1389,7 +1433,7 @@
     <row r="31" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="30"/>
       <c r="B31" s="25"/>
-      <c r="C31" s="42">
+      <c r="C31" s="41">
         <f>C29/C30</f>
         <v>0.15883768563311068</v>
       </c>
@@ -1420,60 +1464,305 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="2">
+      <c r="A1" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="42">
+        <v>2013</v>
+      </c>
+      <c r="C2" s="43">
+        <v>993160200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="42">
+        <v>2013</v>
+      </c>
+      <c r="C3" s="43">
+        <v>2165466600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="42">
+        <v>2013</v>
+      </c>
+      <c r="C4" s="43">
+        <v>2700078240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="44">
+        <v>2013</v>
+      </c>
+      <c r="C5" s="45">
+        <v>217889760</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C6" s="39">
+        <f>SUM(C2:C5)</f>
+        <v>6076594800</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B1" s="2">
-        <v>2013</v>
-      </c>
-      <c r="C1" s="32">
-        <v>993160200</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>2</v>
-      </c>
       <c r="B2" s="2">
-        <v>2013</v>
-      </c>
-      <c r="C2" s="32">
-        <v>2165466600</v>
+        <v>2009</v>
+      </c>
+      <c r="C2" s="2">
+        <v>817399900</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>2013</v>
-      </c>
-      <c r="C3" s="32">
-        <v>2700078240</v>
+        <v>2010</v>
+      </c>
+      <c r="C3" s="2">
+        <v>843487120</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2011</v>
+      </c>
+      <c r="C4" s="2">
+        <v>907002080</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2012</v>
+      </c>
+      <c r="C5" s="2">
+        <v>949344840</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2013</v>
+      </c>
+      <c r="C6" s="2">
+        <v>993160200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2009</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1578091680</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2010</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1647202920</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2011</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1844013700</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2012</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2044201080</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2013</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2165466600</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2009</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2335745420</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2010</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2404117630</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2011</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2459521140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2012</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2529970500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2013</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2700078240</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
-        <v>2013</v>
-      </c>
-      <c r="C4" s="32">
-        <v>217889760</v>
+      <c r="B17" s="2">
+        <v>2009</v>
+      </c>
+      <c r="C17" s="2">
+        <v>163737360</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>4</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2010</v>
+      </c>
+      <c r="C18" s="2">
+        <v>152995920</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>4</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2011</v>
+      </c>
+      <c r="C19" s="2">
+        <v>184134720</v>
       </c>
     </row>
   </sheetData>

</xml_diff>